<commit_message>
renamed Testcases-dir to Section14 and added a DataDriven test
</commit_message>
<xml_diff>
--- a/Resources/testdata.xlsx
+++ b/Resources/testdata.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurikyttala/coding/Udemy_Rahul_Arora_RF/Section8/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurikyttala/coding/Udemy_Rahul_Arora_RF/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8712256E-7805-5541-9FF8-D34E60C4753B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DFEBE71-1A16-E942-81D3-6C548A6E75A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="0" windowWidth="25240" windowHeight="17440" xr2:uid="{4C5BED7A-655E-5A4D-9346-A63876D5259C}"/>
+    <workbookView xWindow="11220" yWindow="0" windowWidth="17180" windowHeight="17440" activeTab="1" xr2:uid="{4C5BED7A-655E-5A4D-9346-A63876D5259C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FindNewCarTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>${month}</t>
   </si>
@@ -54,6 +55,36 @@
   </si>
   <si>
     <t>December</t>
+  </si>
+  <si>
+    <t>${browser}</t>
+  </si>
+  <si>
+    <t>${brandname}</t>
+  </si>
+  <si>
+    <t>${carheading}</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>toyota</t>
+  </si>
+  <si>
+    <t>kia</t>
+  </si>
+  <si>
+    <t>bmw</t>
+  </si>
+  <si>
+    <t>Kia Cars</t>
+  </si>
+  <si>
+    <t>Toyta Cars</t>
+  </si>
+  <si>
+    <t>BMW Cars</t>
   </si>
 </sst>
 </file>
@@ -407,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D172E9-4CCF-9C4A-9463-14109E11A37F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -456,4 +487,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A764EB80-FD11-2743-BE44-6CB4525E13B5}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added GetCarNameTest + some Readme comments
</commit_message>
<xml_diff>
--- a/Resources/testdata.xlsx
+++ b/Resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurikyttala/coding/Udemy_Rahul_Arora_RF/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DFEBE71-1A16-E942-81D3-6C548A6E75A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1226D82C-AF47-7F47-9CA9-325C64927614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="0" windowWidth="17180" windowHeight="17440" activeTab="1" xr2:uid="{4C5BED7A-655E-5A4D-9346-A63876D5259C}"/>
+    <workbookView xWindow="-19620" yWindow="2580" windowWidth="17180" windowHeight="17440" activeTab="1" xr2:uid="{4C5BED7A-655E-5A4D-9346-A63876D5259C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,10 +81,10 @@
     <t>Kia Cars</t>
   </si>
   <si>
-    <t>Toyta Cars</t>
-  </si>
-  <si>
     <t>BMW Cars</t>
+  </si>
+  <si>
+    <t>Toyota Cars</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,7 +522,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -544,7 +544,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>